<commit_message>
#noissue -re organize algorithm
</commit_message>
<xml_diff>
--- a/Doc/data.xlsx
+++ b/Doc/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1100" windowWidth="31060" windowHeight="19820"/>
+    <workbookView xWindow="10940" yWindow="1680" windowWidth="31060" windowHeight="19820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>R(objective function, Rij)</t>
+  </si>
+  <si>
+    <t>RC</t>
+  </si>
+  <si>
+    <t>Sigma</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
@@ -3355,1937 +3361,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-      <c r="J1">
-        <v>0</v>
-      </c>
-      <c r="K1">
-        <v>0</v>
-      </c>
-      <c r="L1">
-        <v>0</v>
-      </c>
-      <c r="M1">
-        <v>0</v>
-      </c>
-      <c r="N1">
-        <v>0</v>
-      </c>
-      <c r="O1">
-        <v>0</v>
-      </c>
-      <c r="P1">
-        <v>0</v>
-      </c>
-      <c r="Q1">
-        <v>0</v>
-      </c>
-      <c r="R1">
-        <v>0</v>
-      </c>
-      <c r="S1">
-        <v>0</v>
-      </c>
-      <c r="T1">
-        <v>0</v>
-      </c>
-      <c r="U1">
-        <v>0</v>
-      </c>
-      <c r="V1">
-        <v>0</v>
-      </c>
-      <c r="W1">
-        <v>0</v>
-      </c>
-      <c r="X1">
-        <v>0</v>
-      </c>
-      <c r="Y1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>0</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
-      <c r="X13">
-        <v>0</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
-      </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <v>0</v>
-      </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="W16">
-        <v>0</v>
-      </c>
-      <c r="X16">
-        <v>0</v>
-      </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
-      <c r="X19">
-        <v>0</v>
-      </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
-      <c r="X20">
-        <v>0</v>
-      </c>
-      <c r="Y20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-      <c r="Y21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22">
-        <v>0</v>
-      </c>
-      <c r="X22">
-        <v>0</v>
-      </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>0</v>
-      </c>
-      <c r="V23">
-        <v>0</v>
-      </c>
-      <c r="W23">
-        <v>0</v>
-      </c>
-      <c r="X23">
-        <v>0</v>
-      </c>
-      <c r="Y23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>0</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>0</v>
-      </c>
-      <c r="V24">
-        <v>0</v>
-      </c>
-      <c r="W24">
-        <v>0</v>
-      </c>
-      <c r="X24">
-        <v>0</v>
-      </c>
-      <c r="Y24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
-      <c r="T25">
-        <v>0</v>
-      </c>
-      <c r="U25">
-        <v>0</v>
-      </c>
-      <c r="V25">
-        <v>0</v>
-      </c>
-      <c r="W25">
-        <v>0</v>
-      </c>
-      <c r="X25">
-        <v>0</v>
-      </c>
-      <c r="Y25">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>